<commit_message>
api controller a and chem iso
</commit_message>
<xml_diff>
--- a/frontend/modules/reports/modules/lab/templates/CHEM_ISO.xlsx
+++ b/frontend/modules/reports/modules/lab/templates/CHEM_ISO.xlsx
@@ -369,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -455,6 +455,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +554,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="88900" y="158750"/>
-          <a:ext cx="603250" cy="442384"/>
+          <a:ext cx="600075" cy="437622"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -989,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="50" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1002,28 +1003,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
@@ -1310,7 +1311,10 @@
       <c r="D52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>

</xml_diff>